<commit_message>
[NguyenPT][Review] Review and add comment
</commit_message>
<xml_diff>
--- a/Document/Investigate/AlaProject_InvestigateListFunctionHaiVL_HienTP.xlsx
+++ b/Document/Investigate/AlaProject_InvestigateListFunctionHaiVL_HienTP.xlsx
@@ -1,22 +1,106 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="4170"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="4170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List Function HaiVL" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>NguyenPT</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>NguyenPT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Anh không thấy chỗ "bị trùng" với "báo cáo".
+Nếu em đưa ra hình ảnh thì trực quan hơn</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>NguyenPT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bổ sung thêm các thành phần (control) trên trang đăng ảnh, ví dụ: Textbox điền tiêu đề, Check box ảnh tự làm, Textbox nguồn của ảnh, Button chọn ảnh, Khung Preview ảnh, Button Đăng ảnh</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NguyenPT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Anh thấy ko có chức năng này trên app HaiVL.
+Có lẽ em hiểu nhầm task rồi, không phải là investigate website haivl.com, mà là investigate app haivl trên android</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>List Function HaiVL</t>
   </si>
@@ -106,12 +190,40 @@
   <si>
     <t>Xem ảnh (mới/hot/chưa xem/cũ/comment)</t>
   </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Xem mới</t>
+  </si>
+  <si>
+    <t>- Button Menu
+- Image Haivl logo
+- Button Reload
+- Image
+- Title image
+- Like number
+- Button comment and Comment number
+- …</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,8 +254,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,8 +294,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -217,11 +361,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,6 +411,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -265,6 +436,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2857144</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4100001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Screenshot_2014-08-10-14-07-36.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2343151" y="190500"/>
+          <a:ext cx="2857143" cy="4100001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,7 +556,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -377,7 +590,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -553,21 +765,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="47.42578125" customWidth="1"/>
     <col min="3" max="3" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:4" ht="30.75" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -575,8 +787,8 @@
       <c r="C2" s="10"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -587,7 +799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="105.75" thickBot="1">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -598,7 +810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -609,7 +821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -620,7 +832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -631,7 +843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -642,7 +854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -653,7 +865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -664,7 +876,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -675,7 +887,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -686,14 +898,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="16.5" thickBot="1">
       <c r="A14" s="3"/>
       <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -704,7 +916,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="75.75" thickBot="1">
       <c r="A16" s="3">
         <v>2</v>
       </c>
@@ -721,28 +933,312 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="12" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="59.42578125" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="326.25" customHeight="1">
+      <c r="A2" s="13">
+        <f>IF(B2="","",ROW()-ROW($A$1))</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="13" t="str">
+        <f t="shared" ref="A3:A26" si="0">IF(B3="","",ROW()-ROW($A$1))</f>
+        <v/>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>